<commit_message>
Added SemanticUI files :heart:
</commit_message>
<xml_diff>
--- a/ExpenseCopy1.xlsx
+++ b/ExpenseCopy1.xlsx
@@ -37,9 +37,6 @@
     <t>Employee Name:</t>
   </si>
   <si>
-    <t>Sammi</t>
-  </si>
-  <si>
     <t>Daytime Phone Number:</t>
   </si>
   <si>
@@ -50,9 +47,6 @@
   </si>
   <si>
     <t>Email Address:</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>Mileage Rate Per Policy</t>
@@ -130,6 +124,12 @@
   </si>
   <si>
     <t>Code</t>
+  </si>
+  <si>
+    <t>08/08/1996</t>
+  </si>
+  <si>
+    <t>Example</t>
   </si>
   <si>
     <t xml:space="preserve"> TOTALS </t>
@@ -1818,24 +1818,20 @@
       </c>
       <c r="B4" s="82"/>
       <c r="C4" s="82"/>
-      <c r="D4" s="83" t="s">
-        <v>6</v>
-      </c>
+      <c r="D4" s="83"/>
       <c r="E4" s="83"/>
       <c r="F4" s="83"/>
       <c r="G4" s="84" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H4" s="85"/>
       <c r="I4" s="85"/>
-      <c r="J4" s="86">
-        <v>333</v>
-      </c>
+      <c r="J4" s="86"/>
       <c r="K4" s="86"/>
       <c r="L4" s="86"/>
       <c r="M4" s="3"/>
       <c r="N4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
@@ -1849,23 +1845,19 @@
     </row>
     <row r="5" spans="1:23" customHeight="1" ht="25.5">
       <c r="A5" s="82" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="82"/>
       <c r="C5" s="82"/>
-      <c r="D5" s="89">
-        <v>333</v>
-      </c>
+      <c r="D5" s="89"/>
       <c r="E5" s="89"/>
       <c r="F5" s="89"/>
       <c r="G5" s="92" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H5" s="93"/>
       <c r="I5" s="93"/>
-      <c r="J5" s="89" t="s">
-        <v>11</v>
-      </c>
+      <c r="J5" s="89"/>
       <c r="K5" s="89"/>
       <c r="L5" s="89"/>
       <c r="M5" s="3"/>
@@ -1890,7 +1882,7 @@
       <c r="H6" s="91"/>
       <c r="I6" s="91"/>
       <c r="J6" s="91" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K6" s="91"/>
       <c r="L6" s="91"/>
@@ -1929,13 +1921,13 @@
     </row>
     <row r="8" spans="1:23" customHeight="1" ht="25.5">
       <c r="A8" s="90" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="90"/>
       <c r="C8" s="90"/>
       <c r="D8" s="90"/>
       <c r="E8" s="87" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F8" s="87"/>
       <c r="G8" s="87"/>
@@ -1957,7 +1949,7 @@
       <c r="C9" s="90"/>
       <c r="D9" s="90"/>
       <c r="E9" s="88" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F9" s="88"/>
       <c r="G9" s="88"/>
@@ -1976,10 +1968,10 @@
     </row>
     <row r="10" spans="1:23" customHeight="1" ht="22.5">
       <c r="A10" s="121" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="135" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="135"/>
       <c r="D10" s="135"/>
@@ -2001,31 +1993,31 @@
     <row r="11" spans="1:23" customHeight="1" ht="22.5">
       <c r="A11" s="121"/>
       <c r="B11" s="143" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="101" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" s="101"/>
       <c r="E11" s="105" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="101" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="101" t="s">
+      <c r="H11" s="105" t="s">
         <v>21</v>
-      </c>
-      <c r="G11" s="101" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="105" t="s">
-        <v>23</v>
       </c>
       <c r="I11" s="105"/>
       <c r="J11" s="105" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K11" s="105"/>
       <c r="L11" s="139" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -2043,16 +2035,16 @@
       <c r="F12" s="102"/>
       <c r="G12" s="102"/>
       <c r="H12" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="J12" s="42" t="s">
-        <v>28</v>
-      </c>
       <c r="K12" s="42" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L12" s="140"/>
       <c r="M12" s="3"/>
@@ -2068,24 +2060,16 @@
         <v>0</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C13" s="98" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D13" s="98"/>
-      <c r="E13" s="4">
-        <v>3</v>
-      </c>
-      <c r="F13" s="4">
-        <v>3</v>
-      </c>
-      <c r="G13" s="4">
-        <v>3</v>
-      </c>
-      <c r="H13" s="22">
-        <v>3</v>
-      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="22"/>
       <c r="I13" s="21" t="str">
         <f>ROUND((H13*$J$7),2)</f>
         <v>0</v>
@@ -2226,7 +2210,7 @@
     </row>
     <row r="19" spans="1:23" customHeight="1" ht="22.5">
       <c r="A19" s="120" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" s="106" t="s">
         <v>30</v>
@@ -2245,31 +2229,31 @@
     <row r="20" spans="1:23" customHeight="1" ht="22.5">
       <c r="A20" s="121"/>
       <c r="B20" s="143" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C20" s="101" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D20" s="101"/>
       <c r="E20" s="105" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="101" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="101" t="s">
+      <c r="H20" s="105" t="s">
         <v>21</v>
-      </c>
-      <c r="G20" s="101" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="105" t="s">
-        <v>23</v>
       </c>
       <c r="I20" s="105"/>
       <c r="J20" s="105" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K20" s="105"/>
       <c r="L20" s="137" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:23" customHeight="1" ht="22.5">
@@ -2281,16 +2265,16 @@
       <c r="F21" s="102"/>
       <c r="G21" s="102"/>
       <c r="H21" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="I21" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="J21" s="42" t="s">
-        <v>28</v>
-      </c>
       <c r="K21" s="42" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L21" s="138"/>
     </row>
@@ -2422,7 +2406,7 @@
     </row>
     <row r="27" spans="1:23" customHeight="1" ht="22.5">
       <c r="A27" s="120" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B27" s="135" t="s">
         <v>31</v>
@@ -2441,10 +2425,10 @@
     <row r="28" spans="1:23" customHeight="1" ht="22.5">
       <c r="A28" s="121"/>
       <c r="B28" s="109" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C28" s="105" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D28" s="105"/>
       <c r="E28" s="105"/>
@@ -2452,14 +2436,14 @@
       <c r="G28" s="105"/>
       <c r="H28" s="105"/>
       <c r="I28" s="101" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J28" s="105" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K28" s="105"/>
       <c r="L28" s="137" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:23" customHeight="1" ht="22.5">
@@ -2473,10 +2457,10 @@
       <c r="H29" s="116"/>
       <c r="I29" s="102"/>
       <c r="J29" s="42" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K29" s="42" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L29" s="138"/>
     </row>
@@ -2587,7 +2571,7 @@
     </row>
     <row r="35" spans="1:23" customHeight="1" ht="22.5">
       <c r="A35" s="120" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B35" s="106" t="s">
         <v>32</v>
@@ -2606,7 +2590,7 @@
     <row r="36" spans="1:23" customHeight="1" ht="32.25">
       <c r="A36" s="121"/>
       <c r="B36" s="56" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C36" s="116" t="s">
         <v>33</v>
@@ -2620,7 +2604,7 @@
       <c r="J36" s="116"/>
       <c r="K36" s="116"/>
       <c r="L36" s="57" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O36" s="3"/>
     </row>

</xml_diff>